<commit_message>
did some tuning on sha256 and improved test bench uploaded binary files in docs folder added common file for hmac_sha256_x functions
</commit_message>
<xml_diff>
--- a/docs/Design_Budgeting_Form.xlsx
+++ b/docs/Design_Budgeting_Form.xlsx
@@ -14,13 +14,14 @@
   <definedNames>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Area Budget'!$A$1:$E$32</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Area Budget'!$A$1:$E$32</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">'Area Budget'!$A$1:$E$32</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="65">
   <si>
     <t>Core Area Calculations</t>
   </si>
@@ -89,64 +90,61 @@
     <t>Combinational</t>
   </si>
   <si>
-    <t>Scratchpad SRAM</t>
+    <t>Scratchpad SRAM, slide 13</t>
   </si>
   <si>
     <t>Majority of space. Can move off-chip to reduce</t>
   </si>
   <si>
-    <t>Blockmix Input Register</t>
-  </si>
-  <si>
-    <t>Storage register for blockmix input</t>
-  </si>
-  <si>
-    <t>PBKDF2_1 Input Register</t>
-  </si>
-  <si>
-    <t>storage register for pbkdf2 message input</t>
-  </si>
-  <si>
-    <t>PBKDF2_2 Input Register</t>
-  </si>
-  <si>
-    <t>Salsa20/8 logic</t>
-  </si>
-  <si>
-    <t>Combinational logic for each salsa20/8 operation</t>
-  </si>
-  <si>
-    <t>SMIX 128B bitwise XOR</t>
-  </si>
-  <si>
-    <t>Input to BLOCKMIX in second round</t>
-  </si>
-  <si>
-    <t>BLOCKMIX 64B bitwise XOR</t>
-  </si>
-  <si>
-    <t>Input to Salsa20/8</t>
-  </si>
-  <si>
-    <t>Block 80B SRAM</t>
-  </si>
-  <si>
-    <t>Storage for message to hash</t>
-  </si>
-  <si>
-    <t>UART FSM/Buffer/Timer</t>
-  </si>
-  <si>
-    <t>UART registers</t>
-  </si>
-  <si>
-    <t>Controller FSM/Timer</t>
-  </si>
-  <si>
-    <t>Controller FSM register</t>
-  </si>
-  <si>
-    <t>Cycle Decoder</t>
+    <t>8x(SHA256 w,a..h,hash registers), slide 12</t>
+  </si>
+  <si>
+    <t>Registers for SHA algorithm</t>
+  </si>
+  <si>
+    <t>8x(SHA256 state,round registers), slide 12</t>
+  </si>
+  <si>
+    <t>State and counter for SHA algorithm</t>
+  </si>
+  <si>
+    <t>8x(HMAC counter), slide 10/11</t>
+  </si>
+  <si>
+    <t>Counter for HMAC logic</t>
+  </si>
+  <si>
+    <t>8x(HMAC combinational), slide 10/11</t>
+  </si>
+  <si>
+    <t>Combinational logic for HMAC blocks</t>
+  </si>
+  <si>
+    <t>4x(HMAC buffer), slide 10/11</t>
+  </si>
+  <si>
+    <t>Data buffer for use in HMAC algorithm</t>
+  </si>
+  <si>
+    <t>Scrypt Data Copy, slide 7</t>
+  </si>
+  <si>
+    <t>Copy of input data for scrypt block</t>
+  </si>
+  <si>
+    <t>SMIX state and counter, slide 13</t>
+  </si>
+  <si>
+    <t>Blockmix X register, slide 14</t>
+  </si>
+  <si>
+    <t>Salsa data register, slide 15</t>
+  </si>
+  <si>
+    <t>Top-Level SRAM, slide 4</t>
+  </si>
+  <si>
+    <t>SRAM to store incoming block data</t>
   </si>
   <si>
     <t>Total Core Area</t>
@@ -195,9 +193,6 @@
     <t>Core Dimensions</t>
   </si>
   <si>
-    <t>by </t>
-  </si>
-  <si>
     <t>Core Based Padframe Dimensions:</t>
   </si>
   <si>
@@ -228,22 +223,22 @@
     <t>Target Clock Period (ns)</t>
   </si>
   <si>
-    <t>controller hash_cycle FSM output</t>
-  </si>
-  <si>
-    <t>cycle decoder, mux &amp; input padder</t>
-  </si>
-  <si>
-    <t>BLOCKMIX input register</t>
-  </si>
-  <si>
-    <t>Salsa20/8 X register output</t>
-  </si>
-  <si>
-    <t>xor, add, rot</t>
-  </si>
-  <si>
-    <t>Salsa20/8 X register input</t>
+    <t>SHA compression a</t>
+  </si>
+  <si>
+    <t>rot, xor, add, add</t>
+  </si>
+  <si>
+    <t>a register input</t>
+  </si>
+  <si>
+    <t>Salsa20/8 data register output</t>
+  </si>
+  <si>
+    <t>xor, add, rot, mux</t>
+  </si>
+  <si>
+    <t>Salsa20/8 data register input</t>
   </si>
   <si>
     <t>SHA compression e</t>
@@ -255,10 +250,22 @@
     <t>SHA compression d</t>
   </si>
   <si>
-    <t>SHA compression a</t>
-  </si>
-  <si>
-    <t>rot, xor, add, add</t>
+    <t>Top-level SRAM</t>
+  </si>
+  <si>
+    <t>mux/padder</t>
+  </si>
+  <si>
+    <t>SHA256 input</t>
+  </si>
+  <si>
+    <t>Scratchpad SRAM</t>
+  </si>
+  <si>
+    <t>mux</t>
+  </si>
+  <si>
+    <t>SMIX X input</t>
   </si>
 </sst>
 </file>
@@ -492,7 +499,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="38">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
@@ -577,10 +584,6 @@
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="7" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
     <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="9" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
@@ -595,10 +598,6 @@
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="10" fillId="0" fontId="0" numFmtId="166" xfId="15">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="8" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="11" fillId="0" fontId="0" numFmtId="166" xfId="15">
@@ -673,12 +672,12 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="D33" activeCellId="0" pane="topLeft" sqref="D33"/>
+      <selection activeCell="A18" activeCellId="0" pane="topLeft" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="31.280612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="47.6428571428571"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.8571428571429"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="1" width="11.8622448979592"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="17"/>
@@ -794,7 +793,7 @@
         <v>15</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.15" outlineLevel="0" r="8">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="8">
       <c r="A8" s="8" t="s">
         <v>16</v>
       </c>
@@ -802,183 +801,181 @@
         <v>9</v>
       </c>
       <c r="C8" s="8" t="n">
+        <f aca="false">8*(64*32+256+256)</f>
+        <v>20480</v>
+      </c>
+      <c r="D8" s="9" t="n">
+        <f aca="false">IF(B8="Combinational",C8*500*1.5,IF(B8="Reg. w/ Reset",C8*1600*1.5,IF(B8="Reg. w/o Reset",C8*900*1.5,IF(B8="On-chip SRAM",C8*50*1.5,"N/A"))))</f>
+        <v>27648000</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="9">
+      <c r="A9" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="8" t="n">
+        <f aca="false">8*(7+3)</f>
+        <v>80</v>
+      </c>
+      <c r="D9" s="9" t="n">
+        <f aca="false">IF(B9="Combinational",C9*500*1.5,IF(B9="Reg. w/ Reset",C9*1600*1.5,IF(B9="Reg. w/o Reset",C9*900*1.5,IF(B9="On-chip SRAM",C9*50*1.5,"N/A"))))</f>
+        <v>192000</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="10">
+      <c r="A10" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="8" t="n">
+        <f aca="false">8*(2)</f>
+        <v>16</v>
+      </c>
+      <c r="D10" s="9" t="n">
+        <f aca="false">IF(B10="Combinational",C10*500*1.5,IF(B10="Reg. w/ Reset",C10*1600*1.5,IF(B10="Reg. w/o Reset",C10*900*1.5,IF(B10="On-chip SRAM",C10*50*1.5,"N/A"))))</f>
+        <v>38400</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.15" outlineLevel="0" r="11">
+      <c r="A11" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="8" t="n">
+        <f aca="false">8*(4)</f>
+        <v>32</v>
+      </c>
+      <c r="D11" s="9" t="n">
+        <f aca="false">IF(B11="Combinational",C11*500*1.5,IF(B11="Reg. w/ Reset",C11*1600*1.5,IF(B11="Reg. w/o Reset",C11*900*1.5,IF(B11="On-chip SRAM",C11*50*1.5,"N/A"))))</f>
+        <v>24000</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="12">
+      <c r="A12" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="8" t="n">
+        <f aca="false">4*(32*8)</f>
+        <v>1024</v>
+      </c>
+      <c r="D12" s="9" t="n">
+        <f aca="false">IF(B12="Combinational",C12*500*1.5,IF(B12="Reg. w/ Reset",C12*1600*1.5,IF(B12="Reg. w/o Reset",C12*900*1.5,IF(B12="On-chip SRAM",C12*50*1.5,"N/A"))))</f>
+        <v>1382400</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.15" outlineLevel="0" r="13">
+      <c r="A13" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="8" t="n">
+        <f aca="false">80*8</f>
+        <v>640</v>
+      </c>
+      <c r="D13" s="9" t="n">
+        <f aca="false">IF(B13="Combinational",C13*500*1.5,IF(B13="Reg. w/ Reset",C13*1600*1.5,IF(B13="Reg. w/o Reset",C13*900*1.5,IF(B13="On-chip SRAM",C13*50*1.5,"N/A"))))</f>
+        <v>864000</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="14">
+      <c r="A14" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="8" t="n">
+        <f aca="false">10+3</f>
+        <v>13</v>
+      </c>
+      <c r="D14" s="9" t="n">
+        <f aca="false">IF(B14="Combinational",C14*500*1.5,IF(B14="Reg. w/ Reset",C14*1600*1.5,IF(B14="Reg. w/o Reset",C14*900*1.5,IF(B14="On-chip SRAM",C14*50*1.5,"N/A"))))</f>
+        <v>31200</v>
+      </c>
+      <c r="E14" s="10"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.15" outlineLevel="0" r="15">
+      <c r="A15" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="8" t="n">
         <f aca="false">128*8</f>
         <v>1024</v>
       </c>
-      <c r="D8" s="9" t="n">
-        <f aca="false">IF(B8="Combinational",C8*500*1.5,IF(B8="Reg. w/ Reset",C8*1600*1.5,IF(B8="Reg. w/o Reset",C8*900*1.5,IF(B8="On-chip SRAM",C8*50*1.5,"N/A"))))</f>
+      <c r="D15" s="9" t="n">
+        <f aca="false">IF(B15="Combinational",C15*500*1.5,IF(B15="Reg. w/ Reset",C15*1600*1.5,IF(B15="Reg. w/o Reset",C15*900*1.5,IF(B15="On-chip SRAM",C15*50*1.5,"N/A"))))</f>
         <v>1382400</v>
       </c>
-      <c r="E8" s="10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="9">
-      <c r="A9" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="8" t="s">
+      <c r="E15" s="10"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="16">
+      <c r="A16" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="8" t="n">
-        <f aca="false">160*8</f>
-        <v>1280</v>
-      </c>
-      <c r="D9" s="9" t="n">
-        <f aca="false">IF(B9="Combinational",C9*500*1.5,IF(B9="Reg. w/ Reset",C9*1600*1.5,IF(B9="Reg. w/o Reset",C9*900*1.5,IF(B9="On-chip SRAM",C9*50*1.5,"N/A"))))</f>
-        <v>1728000</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="10">
-      <c r="A10" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="8" t="n">
-        <f aca="false">(128+80)*8</f>
-        <v>1664</v>
-      </c>
-      <c r="D10" s="9" t="n">
-        <f aca="false">IF(B10="Combinational",C10*500*1.5,IF(B10="Reg. w/ Reset",C10*1600*1.5,IF(B10="Reg. w/o Reset",C10*900*1.5,IF(B10="On-chip SRAM",C10*50*1.5,"N/A"))))</f>
-        <v>2246400</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.15" outlineLevel="0" r="11">
-      <c r="A11" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="8" t="n">
-        <f aca="false">32*3</f>
-        <v>96</v>
-      </c>
-      <c r="D11" s="9" t="n">
-        <f aca="false">IF(B11="Combinational",C11*500*1.5,IF(B11="Reg. w/ Reset",C11*1600*1.5,IF(B11="Reg. w/o Reset",C11*900*1.5,IF(B11="On-chip SRAM",C11*50*1.5,"N/A"))))</f>
-        <v>72000</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.15" outlineLevel="0" r="12">
-      <c r="A12" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" s="8" t="n">
-        <f aca="false">128*8</f>
-        <v>1024</v>
-      </c>
-      <c r="D12" s="9" t="n">
-        <f aca="false">IF(B12="Combinational",C12*500*1.5,IF(B12="Reg. w/ Reset",C12*1600*1.5,IF(B12="Reg. w/o Reset",C12*900*1.5,IF(B12="On-chip SRAM",C12*50*1.5,"N/A"))))</f>
-        <v>768000</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.15" outlineLevel="0" r="13">
-      <c r="A13" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="8" t="n">
-        <f aca="false">64*8</f>
+      <c r="C16" s="8" t="n">
+        <f aca="false">8*64</f>
         <v>512</v>
       </c>
-      <c r="D13" s="9" t="n">
-        <f aca="false">IF(B13="Combinational",C13*500*1.5,IF(B13="Reg. w/ Reset",C13*1600*1.5,IF(B13="Reg. w/o Reset",C13*900*1.5,IF(B13="On-chip SRAM",C13*50*1.5,"N/A"))))</f>
-        <v>384000</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="14">
-      <c r="A14" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="B14" s="8" t="s">
+      <c r="D16" s="9" t="n">
+        <f aca="false">IF(B16="Combinational",C16*500*1.5,IF(B16="Reg. w/ Reset",C16*1600*1.5,IF(B16="Reg. w/o Reset",C16*900*1.5,IF(B16="On-chip SRAM",C16*50*1.5,"N/A"))))</f>
+        <v>691200</v>
+      </c>
+      <c r="E16" s="10"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="17">
+      <c r="A17" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="8" t="n">
+      <c r="C17" s="8" t="n">
         <f aca="false">80*8</f>
         <v>640</v>
       </c>
-      <c r="D14" s="9" t="n">
-        <f aca="false">IF(B14="Combinational",C14*500*1.5,IF(B14="Reg. w/ Reset",C14*1600*1.5,IF(B14="Reg. w/o Reset",C14*900*1.5,IF(B14="On-chip SRAM",C14*50*1.5,"N/A"))))</f>
-        <v>48000</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="15">
-      <c r="A15" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C15" s="8" t="n">
-        <f aca="false">9+10+16</f>
-        <v>35</v>
-      </c>
-      <c r="D15" s="9" t="n">
-        <f aca="false">IF(B15="Combinational",C15*500*1.5,IF(B15="Reg. w/ Reset",C15*1600*1.5,IF(B15="Reg. w/o Reset",C15*900*1.5,IF(B15="On-chip SRAM",C15*50*1.5,"N/A"))))</f>
-        <v>84000</v>
-      </c>
-      <c r="E15" s="10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="16">
-      <c r="A16" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C16" s="8" t="n">
-        <v>5</v>
-      </c>
-      <c r="D16" s="9" t="n">
-        <f aca="false">IF(B16="Combinational",C16*500*1.5,IF(B16="Reg. w/ Reset",C16*1600*1.5,IF(B16="Reg. w/o Reset",C16*900*1.5,IF(B16="On-chip SRAM",C16*50*1.5,"N/A"))))</f>
-        <v>12000</v>
-      </c>
-      <c r="E16" s="10" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.15" outlineLevel="0" r="17">
-      <c r="A17" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C17" s="8" t="n">
-        <v>5</v>
-      </c>
       <c r="D17" s="9" t="n">
         <f aca="false">IF(B17="Combinational",C17*500*1.5,IF(B17="Reg. w/ Reset",C17*1600*1.5,IF(B17="Reg. w/o Reset",C17*900*1.5,IF(B17="On-chip SRAM",C17*50*1.5,"N/A"))))</f>
-        <v>3750</v>
-      </c>
-      <c r="E17" s="10"/>
+        <v>48000</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="18">
       <c r="A18" s="8"/>
@@ -1042,19 +1039,19 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.75" outlineLevel="0" r="24">
       <c r="A24" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B24" s="12"/>
       <c r="C24" s="12"/>
       <c r="D24" s="9" t="n">
         <f aca="false">SUM(D3:D22)</f>
-        <v>16328550</v>
+        <v>41901600</v>
       </c>
       <c r="E24" s="12"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="18" outlineLevel="0" r="25">
       <c r="A25" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B25" s="13"/>
       <c r="C25" s="13"/>
@@ -1063,7 +1060,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="26">
       <c r="A26" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B26" s="15" t="n">
         <v>5</v>
@@ -1074,13 +1071,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="27">
       <c r="A27" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B27" s="18" t="n">
         <v>90</v>
       </c>
       <c r="C27" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D27" s="20" t="n">
         <v>300</v>
@@ -1089,14 +1086,14 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="28">
       <c r="A28" s="17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B28" s="18" t="n">
         <f aca="false">($B$26/4)*B27+2*D27</f>
         <v>712.5</v>
       </c>
       <c r="C28" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D28" s="20" t="n">
         <f aca="false">($B$26/4)*B27+2*D27</f>
@@ -1105,67 +1102,67 @@
       <c r="E28" s="16"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="29">
-      <c r="A29" s="21" t="s">
-        <v>40</v>
+      <c r="A29" s="17" t="s">
+        <v>39</v>
       </c>
       <c r="B29" s="18" t="n">
         <f aca="false">SQRT($D$24)</f>
-        <v>4040.86005696807</v>
+        <v>6473.14452179155</v>
       </c>
       <c r="C29" s="19" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D29" s="20" t="n">
         <f aca="false">SQRT($D$24)</f>
-        <v>4040.86005696807</v>
+        <v>6473.14452179155</v>
       </c>
       <c r="E29" s="16"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.75" outlineLevel="0" r="30">
-      <c r="A30" s="22" t="s">
-        <v>42</v>
-      </c>
-      <c r="B30" s="23" t="n">
+      <c r="A30" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="B30" s="22" t="n">
         <f aca="false">B29+3*$D$27</f>
-        <v>4940.86005696807</v>
-      </c>
-      <c r="C30" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="D30" s="25" t="n">
+        <v>7373.14452179155</v>
+      </c>
+      <c r="C30" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="D30" s="24" t="n">
         <f aca="false">D29+3*$D$27</f>
-        <v>4940.86005696807</v>
+        <v>7373.14452179155</v>
       </c>
       <c r="E30" s="16"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="31">
-      <c r="A31" s="21" t="s">
-        <v>43</v>
+      <c r="A31" s="17" t="s">
+        <v>41</v>
       </c>
       <c r="B31" s="18" t="n">
         <f aca="false">MAX(B30,B28)</f>
-        <v>4940.86005696807</v>
-      </c>
-      <c r="C31" s="26" t="s">
-        <v>38</v>
-      </c>
-      <c r="D31" s="27" t="n">
+        <v>7373.14452179155</v>
+      </c>
+      <c r="C31" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="D31" s="25" t="n">
         <f aca="false">MAX(D30,D28)</f>
-        <v>4940.86005696807</v>
+        <v>7373.14452179155</v>
       </c>
       <c r="E31" s="16"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.75" outlineLevel="0" r="32">
-      <c r="A32" s="21" t="s">
-        <v>44</v>
-      </c>
-      <c r="B32" s="28" t="n">
+      <c r="A32" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="B32" s="26" t="n">
         <f aca="false">B31*D31</f>
-        <v>24412098.1025425</v>
-      </c>
-      <c r="C32" s="28"/>
-      <c r="D32" s="28"/>
-      <c r="E32" s="29"/>
+        <v>54363260.1392248</v>
+      </c>
+      <c r="C32" s="26"/>
+      <c r="D32" s="26"/>
+      <c r="E32" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1189,10 +1186,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="C9" activeCellId="0" pane="topLeft" sqref="C9"/>
+      <selection activeCell="A3" activeCellId="0" pane="topLeft" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1208,176 +1205,173 @@
     <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.72959183673469"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="31.5" outlineLevel="0" r="1" s="33">
-      <c r="A1" s="30" t="s">
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="31.5" outlineLevel="0" r="1" s="31">
+      <c r="A1" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="31" t="s">
+      <c r="D1" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="F1" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="D1" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="E1" s="30" t="s">
+      <c r="G1" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="F1" s="31" t="s">
+      <c r="H1" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="G1" s="32" t="s">
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.15" outlineLevel="0" r="2">
+      <c r="A2" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="H1" s="32" t="s">
+      <c r="B2" s="33" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C2" s="32" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="42.4" outlineLevel="0" r="2">
-      <c r="A2" s="34" t="s">
+      <c r="D2" s="33" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E2" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="B2" s="35" t="n">
+      <c r="F2" s="33" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="G2" s="34" t="n">
+        <f aca="false">SUM(F2,B2,D2)</f>
+        <v>0.8</v>
+      </c>
+      <c r="H2" s="34" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="28.75" outlineLevel="0" r="3">
+      <c r="A3" s="35" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" s="36" t="n">
         <v>0.1</v>
       </c>
-      <c r="C2" s="34" t="s">
-        <v>53</v>
-      </c>
-      <c r="D2" s="35" t="n">
+      <c r="C3" s="35" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3" s="36" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E3" s="35" t="s">
+        <v>55</v>
+      </c>
+      <c r="F3" s="36" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="G3" s="34" t="n">
+        <f aca="false">SUM(F3,B3,D3)</f>
+        <v>0.8</v>
+      </c>
+      <c r="H3" s="37" t="n">
+        <f aca="false">H2</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="28.75" outlineLevel="0" r="4">
+      <c r="A4" s="35" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" s="36" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C4" s="35" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" s="36" t="n">
         <f aca="false">0.2*5</f>
         <v>1</v>
       </c>
-      <c r="E2" s="34" t="s">
-        <v>54</v>
-      </c>
-      <c r="F2" s="35" t="n">
+      <c r="E4" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="F4" s="36" t="n">
         <v>0.2</v>
       </c>
-      <c r="G2" s="36" t="n">
-        <f aca="false">SUM(F2,B2,D2)</f>
-        <v>1.3</v>
-      </c>
-      <c r="H2" s="36" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="28.75" outlineLevel="0" r="3">
-      <c r="A3" s="37" t="s">
-        <v>55</v>
-      </c>
-      <c r="B3" s="38" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="C3" s="37" t="s">
-        <v>56</v>
-      </c>
-      <c r="D3" s="38" t="n">
-        <f aca="false">0.2*2</f>
-        <v>0.4</v>
-      </c>
-      <c r="E3" s="37" t="s">
-        <v>57</v>
-      </c>
-      <c r="F3" s="38" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="G3" s="36" t="n">
-        <f aca="false">SUM(F3,B3,D3)</f>
-        <v>0.7</v>
-      </c>
-      <c r="H3" s="39" t="n">
-        <f aca="false">H2</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="28.75" outlineLevel="0" r="4">
-      <c r="A4" s="37" t="s">
-        <v>58</v>
-      </c>
-      <c r="B4" s="38" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="C4" s="37" t="s">
-        <v>59</v>
-      </c>
-      <c r="D4" s="38" t="n">
-        <f aca="false">0.2*5</f>
-        <v>1</v>
-      </c>
-      <c r="E4" s="37" t="s">
-        <v>60</v>
-      </c>
-      <c r="F4" s="38" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="G4" s="36" t="n">
+      <c r="G4" s="34" t="n">
         <f aca="false">SUM(F4,B4,D4)</f>
         <v>1.3</v>
       </c>
-      <c r="H4" s="39" t="n">
+      <c r="H4" s="37" t="n">
         <f aca="false">H3</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.15" outlineLevel="0" r="5">
+      <c r="A5" s="35" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" s="36" t="n">
         <v>5</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.15" outlineLevel="0" r="5">
-      <c r="A5" s="37" t="s">
+      <c r="C5" s="35" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" s="36" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E5" s="32" t="s">
         <v>61</v>
       </c>
-      <c r="B5" s="38" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="C5" s="37" t="s">
+      <c r="F5" s="36" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="G5" s="34" t="n">
+        <f aca="false">SUM(F5,B5,D5)</f>
+        <v>5.7</v>
+      </c>
+      <c r="H5" s="37" t="n">
+        <f aca="false">H4</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.15" outlineLevel="0" r="6">
+      <c r="A6" s="32" t="s">
         <v>62</v>
       </c>
-      <c r="D5" s="38" t="n">
-        <f aca="false">0.2*3</f>
-        <v>0.6</v>
-      </c>
-      <c r="E5" s="34" t="s">
-        <v>61</v>
-      </c>
-      <c r="F5" s="38" t="n">
+      <c r="B6" s="33" t="n">
+        <v>5</v>
+      </c>
+      <c r="C6" s="32" t="s">
+        <v>63</v>
+      </c>
+      <c r="D6" s="33" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E6" s="32" t="s">
+        <v>64</v>
+      </c>
+      <c r="F6" s="33" t="n">
         <v>0.2</v>
       </c>
-      <c r="G5" s="36" t="n">
-        <f aca="false">SUM(F5,B5,D5)</f>
-        <v>0.9</v>
-      </c>
-      <c r="H5" s="39" t="n">
-        <f aca="false">H4</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.15" outlineLevel="0" r="6">
-      <c r="A6" s="34" t="s">
-        <v>61</v>
-      </c>
-      <c r="B6" s="35" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="C6" s="34" t="s">
-        <v>62</v>
-      </c>
-      <c r="D6" s="35" t="n">
-        <f aca="false">0.2*3</f>
-        <v>0.6</v>
-      </c>
-      <c r="E6" s="34" t="s">
-        <v>61</v>
-      </c>
-      <c r="F6" s="35" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="G6" s="39" t="n">
+      <c r="G6" s="37" t="n">
         <f aca="false">SUM(F6,B6,D6)</f>
-        <v>0.9</v>
-      </c>
-      <c r="H6" s="39" t="n">
+        <v>5.7</v>
+      </c>
+      <c r="H6" s="37" t="n">
         <f aca="false">H5</f>
-        <v>5</v>
-      </c>
-    </row>
+        <v>6</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="7"/>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="8"/>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="9"/>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="10"/>

</xml_diff>